<commit_message>
students enrolled, teachers assigned to course
</commit_message>
<xml_diff>
--- a/Planning NLUs term 4.xlsx
+++ b/Planning NLUs term 4.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectDatabase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -204,6 +212,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -286,7 +297,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,8 +328,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5D9F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCC0DA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -432,6 +455,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -439,7 +484,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -507,6 +552,43 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="77"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="77"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,8 +596,36 @@
     <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFFFCCCC"/>
@@ -524,6 +634,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -816,37 +929,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AI40"/>
+  <dimension ref="A1:AK41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI40" activeCellId="3" sqref="AI25:AJ25 AI31:AJ31 AI37:AJ37 AI40:AJ40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.83203125" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="13" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="34" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="34" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="254.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:37" ht="254.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>25</v>
       </c>
@@ -951,156 +1065,228 @@
       </c>
       <c r="AI1" s="13"/>
     </row>
-    <row r="2" spans="1:35" ht="16" thickBot="1">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:37" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34">
+        <v>1</v>
+      </c>
+      <c r="D2" s="35">
+        <v>2</v>
+      </c>
+      <c r="E2" s="34">
+        <v>3</v>
+      </c>
+      <c r="F2" s="35">
+        <v>4</v>
+      </c>
+      <c r="G2" s="34">
+        <v>5</v>
+      </c>
+      <c r="H2" s="35">
+        <v>6</v>
+      </c>
+      <c r="I2" s="34">
+        <v>7</v>
+      </c>
+      <c r="J2" s="35">
+        <v>8</v>
+      </c>
+      <c r="K2" s="34">
+        <v>9</v>
+      </c>
+      <c r="L2" s="35">
+        <v>10</v>
+      </c>
+      <c r="M2" s="34">
+        <v>11</v>
+      </c>
+      <c r="N2" s="35">
+        <v>12</v>
+      </c>
+      <c r="O2" s="34">
+        <v>13</v>
+      </c>
+      <c r="P2" s="35">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="34">
+        <v>15</v>
+      </c>
+      <c r="R2" s="35">
+        <v>16</v>
+      </c>
+      <c r="S2" s="34">
+        <v>17</v>
+      </c>
+      <c r="T2" s="35">
+        <v>18</v>
+      </c>
+      <c r="U2" s="34">
+        <v>19</v>
+      </c>
+      <c r="V2" s="35">
+        <v>20</v>
+      </c>
+      <c r="W2" s="34">
+        <v>21</v>
+      </c>
+      <c r="X2" s="35">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="34">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="35">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="34">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="35">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="34">
+        <v>27</v>
+      </c>
+      <c r="AD2" s="35">
+        <v>28</v>
+      </c>
+      <c r="AE2" s="34">
+        <v>29</v>
+      </c>
+      <c r="AF2" s="35">
+        <v>30</v>
+      </c>
+      <c r="AG2" s="34">
+        <v>31</v>
+      </c>
+      <c r="AH2" s="35">
+        <v>32</v>
+      </c>
+      <c r="AI2" s="13"/>
+    </row>
+    <row r="3" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="8"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-    </row>
-    <row r="3" spans="1:35" ht="16" thickBot="1">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="M3" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="O3" s="8"/>
+      <c r="P3" s="5"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="U3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="8"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="5"/>
       <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
+      <c r="Z3" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
+      <c r="AB3" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
-      <c r="AE3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="5"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
-    </row>
-    <row r="4" spans="1:35" ht="16" thickBot="1">
-      <c r="A4" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>2</v>
+      <c r="AI3" s="24">
+        <v>42122</v>
+      </c>
+      <c r="AJ3" s="27">
+        <v>0.625</v>
+      </c>
+      <c r="AK3" s="23"/>
+    </row>
+    <row r="4" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="5"/>
+      <c r="P4" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="5"/>
+      <c r="W4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
+      <c r="AE4" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF4" s="5"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
-    </row>
-    <row r="5" spans="1:35" ht="16" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
+      <c r="AI4" s="25">
+        <v>42123</v>
+      </c>
+      <c r="AJ4" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1108,12 +1294,12 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -1130,43 +1316,43 @@
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
-      <c r="AC5" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
       <c r="AF5" s="5"/>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
-    </row>
-    <row r="6" spans="1:35" ht="16" thickBot="1">
-      <c r="A6" s="20" t="s">
+      <c r="AI5" s="24">
+        <v>42124</v>
+      </c>
+      <c r="AJ5" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>21</v>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -1178,43 +1364,53 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
+      <c r="AC6" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
       <c r="AF6" s="5"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
-    </row>
-    <row r="7" spans="1:35" ht="16" thickBot="1">
-      <c r="A7" s="17" t="s">
+      <c r="AI6" s="25">
+        <v>42125</v>
+      </c>
+      <c r="AJ6" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>2</v>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="3"/>
+      <c r="Q7" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="5"/>
@@ -1228,17 +1424,21 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
-    </row>
-    <row r="8" spans="1:35" ht="16" thickBot="1">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="AI7" s="26">
+        <v>42125</v>
+      </c>
+      <c r="AJ7" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1246,57 +1446,57 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="K8" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="R8" s="3"/>
       <c r="S8" s="3"/>
-      <c r="T8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="X8" s="5"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-      <c r="AE8" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE8" s="3"/>
       <c r="AF8" s="5"/>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
-    </row>
-    <row r="9" spans="1:35" ht="16" thickBot="1">
-      <c r="A9" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3"/>
+      <c r="AI8" s="24">
+        <v>42125</v>
+      </c>
+      <c r="AJ8" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1305,49 +1505,61 @@
       <c r="O9" s="3"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="R9" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
+      <c r="T9" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
-      <c r="X9" s="5"/>
+      <c r="X9" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Y9" s="3"/>
-      <c r="Z9" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="5"/>
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
-    </row>
-    <row r="10" spans="1:35" ht="16" thickBot="1">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
+      <c r="AI9" s="25">
+        <v>42128</v>
+      </c>
+      <c r="AJ9" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="3"/>
@@ -1359,22 +1571,32 @@
       <c r="W10" s="3"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
+      <c r="Z10" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
-      <c r="AF10" s="5"/>
+      <c r="AF10" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
-    </row>
-    <row r="11" spans="1:35" ht="16" thickBot="1">
-      <c r="A11" s="20" t="s">
+      <c r="AI10" s="24">
+        <v>42131</v>
+      </c>
+      <c r="AJ10" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>21</v>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1387,12 +1609,12 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="N11" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="O11" s="3"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -1404,19 +1626,25 @@
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
-      <c r="AC11" s="8"/>
+      <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
       <c r="AF11" s="5"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
-    </row>
-    <row r="12" spans="1:35" ht="16" thickBot="1">
-      <c r="A12" s="17" t="s">
+      <c r="AI11" s="25">
+        <v>42132</v>
+      </c>
+      <c r="AJ11" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>2</v>
+      <c r="B12" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1431,16 +1659,14 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="3"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="5"/>
@@ -1448,19 +1674,25 @@
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
+      <c r="AC12" s="8"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="5"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
-    </row>
-    <row r="13" spans="1:35" ht="16" thickBot="1">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
+      <c r="AI12" s="26">
+        <v>42132</v>
+      </c>
+      <c r="AJ12" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1470,25 +1702,21 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P13" s="5"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
+      <c r="U13" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="5"/>
@@ -1498,21 +1726,23 @@
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
-      <c r="AE13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF13" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="5"/>
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
-    </row>
-    <row r="14" spans="1:35" ht="16" thickBot="1">
-      <c r="A14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>2</v>
+      <c r="AI13" s="24">
+        <v>42132</v>
+      </c>
+      <c r="AJ13" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1522,55 +1752,61 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="K14" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="M14" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="O14" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="P14" s="5"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
+      <c r="S14" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
-      <c r="X14" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="X14" s="5"/>
       <c r="Y14" s="3"/>
-      <c r="Z14" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
-      <c r="AB14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="5"/>
+      <c r="AE14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF14" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
-    </row>
-    <row r="15" spans="1:35" ht="16" thickBot="1">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
+      <c r="AI14" s="25">
+        <v>42135</v>
+      </c>
+      <c r="AJ14" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1583,58 +1819,72 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
-      <c r="W15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="X15" s="5"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
+      <c r="Z15" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
+      <c r="AB15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
       <c r="AF15" s="5"/>
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
-    </row>
-    <row r="16" spans="1:35" ht="16" thickBot="1">
+      <c r="AI15" s="24">
+        <v>42136</v>
+      </c>
+      <c r="AJ15" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="T16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
+      <c r="W16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="X16" s="5"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
@@ -1646,45 +1896,41 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
-    </row>
-    <row r="17" spans="1:34" ht="16" thickBot="1">
-      <c r="A17" s="20" t="s">
+      <c r="AI16" s="25">
+        <v>42137</v>
+      </c>
+      <c r="AJ16" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="N17" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="O17" s="3"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -1693,65 +1939,85 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
       <c r="AF17" s="5"/>
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
-    </row>
-    <row r="18" spans="1:34" ht="16" thickBot="1">
-      <c r="A18" s="17" t="s">
+      <c r="AI17" s="25">
+        <v>42146</v>
+      </c>
+      <c r="AJ17" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
+      <c r="AB18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="5"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
-    </row>
-    <row r="19" spans="1:34" ht="16" thickBot="1">
+      <c r="AI18" s="26">
+        <v>42146</v>
+      </c>
+      <c r="AJ18" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>2</v>
@@ -1762,132 +2028,138 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="K19" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L19" s="3"/>
-      <c r="M19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="5"/>
+      <c r="P19" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
-      <c r="AF19" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF19" s="5"/>
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
-    </row>
-    <row r="20" spans="1:34" ht="16" thickBot="1">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
+      <c r="AI19" s="24">
+        <v>42146</v>
+      </c>
+      <c r="AJ19" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" s="3"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
+      <c r="V20" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="W20" s="3"/>
-      <c r="X20" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="X20" s="5"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
+      <c r="Z20" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
       <c r="AE20" s="3"/>
-      <c r="AF20" s="5"/>
+      <c r="AF20" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
-    </row>
-    <row r="21" spans="1:34" ht="16" thickBot="1">
-      <c r="A21" s="20" t="s">
+      <c r="AI20" s="24">
+        <v>42152</v>
+      </c>
+      <c r="AJ20" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="O21" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="P21" s="5"/>
-      <c r="Q21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
-      <c r="X21" s="5"/>
+      <c r="X21" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
@@ -1898,39 +2170,51 @@
       <c r="AF21" s="5"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
-    </row>
-    <row r="22" spans="1:34" ht="16" thickBot="1">
-      <c r="A22" s="17" t="s">
+      <c r="AI21" s="25">
+        <v>42153</v>
+      </c>
+      <c r="AJ21" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="B22" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="F22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
-      <c r="U22" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="5"/>
@@ -1944,62 +2228,76 @@
       <c r="AF22" s="5"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
-    </row>
-    <row r="23" spans="1:34" ht="16" thickBot="1">
-      <c r="A23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
+      <c r="AI22" s="26">
+        <v>42153</v>
+      </c>
+      <c r="AJ22" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="5"/>
+      <c r="P23" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
+      <c r="U23" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="5"/>
       <c r="Y23" s="3"/>
-      <c r="Z23" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
-      <c r="AD23" s="8"/>
-      <c r="AE23" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
       <c r="AF23" s="5"/>
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
-    </row>
-    <row r="24" spans="1:34" ht="16" thickBot="1">
-      <c r="A24" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>2</v>
+      <c r="AI23" s="24">
+        <v>42153</v>
+      </c>
+      <c r="AJ23" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -2016,35 +2314,37 @@
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
-      <c r="U24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V24" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
-      <c r="AD24" s="3"/>
-      <c r="AE24" s="3"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF24" s="5"/>
       <c r="AG24" s="3"/>
-      <c r="AH24" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" ht="16" thickBot="1">
-      <c r="A25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>4</v>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="25">
+        <v>42156</v>
+      </c>
+      <c r="AJ24" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2064,41 +2364,45 @@
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W25" s="3"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="3"/>
-      <c r="Z25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
-      <c r="AD25" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
       <c r="AF25" s="5"/>
       <c r="AG25" s="3"/>
-      <c r="AH25" s="3"/>
-    </row>
-    <row r="26" spans="1:34" ht="16" thickBot="1">
+      <c r="AH25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="24">
+        <v>42157</v>
+      </c>
+      <c r="AJ25" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -2116,32 +2420,42 @@
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
+      <c r="W26" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="X26" s="5"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
+      <c r="Z26" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
+      <c r="AD26" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AE26" s="3"/>
       <c r="AF26" s="5"/>
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
-    </row>
-    <row r="27" spans="1:34" ht="16" thickBot="1">
-      <c r="A27" s="20" t="s">
+      <c r="AI26" s="25">
+        <v>42158</v>
+      </c>
+      <c r="AJ26" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>21</v>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="4" t="s">
         <v>1</v>
       </c>
@@ -2152,13 +2466,9 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="O27" s="3"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
@@ -2174,24 +2484,30 @@
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
-      <c r="AE27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE27" s="3"/>
       <c r="AF27" s="5"/>
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
-    </row>
-    <row r="28" spans="1:34" ht="16" thickBot="1">
-      <c r="A28" s="17" t="s">
+      <c r="AI27" s="25">
+        <v>42159</v>
+      </c>
+      <c r="AJ27" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>2</v>
+      <c r="B28" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E28" s="4" t="s">
         <v>1</v>
       </c>
@@ -2202,43 +2518,47 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O28" s="3"/>
+      <c r="M28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="P28" s="5"/>
       <c r="Q28" s="3"/>
-      <c r="R28" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
-      <c r="V28" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="5"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
-      <c r="AB28" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
-      <c r="AE28" s="3"/>
+      <c r="AE28" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF28" s="5"/>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
-    </row>
-    <row r="29" spans="1:34" ht="16" thickBot="1">
-      <c r="A29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
+      <c r="AI28" s="26">
+        <v>42159</v>
+      </c>
+      <c r="AJ28" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>1</v>
@@ -2255,40 +2575,48 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="8"/>
+      <c r="N29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O29" s="3"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="R29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
       <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
+      <c r="V29" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="W29" s="3"/>
       <c r="X29" s="5"/>
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
+      <c r="AB29" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AC29" s="3"/>
-      <c r="AD29" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
       <c r="AF29" s="5"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
-    </row>
-    <row r="30" spans="1:34" ht="16" thickBot="1">
-      <c r="A30" s="20" t="s">
+      <c r="AI29" s="24">
+        <v>42159</v>
+      </c>
+      <c r="AJ29" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>21</v>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>1</v>
@@ -2301,55 +2629,65 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
+      <c r="O30" s="8"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
+      <c r="S30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="5"/>
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
-      <c r="AA30" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
-      <c r="AD30" s="3"/>
+      <c r="AD30" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AE30" s="3"/>
       <c r="AF30" s="5"/>
       <c r="AG30" s="3"/>
-      <c r="AH30" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:34" ht="16" thickBot="1">
-      <c r="A31" s="17" t="s">
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="25">
+        <v>42160</v>
+      </c>
+      <c r="AJ30" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>2</v>
+      <c r="B31" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="E31" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="J31" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -2366,29 +2704,37 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
+      <c r="AA31" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
       <c r="AE31" s="3"/>
       <c r="AF31" s="5"/>
       <c r="AG31" s="3"/>
-      <c r="AH31" s="3"/>
-    </row>
-    <row r="32" spans="1:34" ht="16" thickBot="1">
-      <c r="A32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
+      <c r="AH31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI31" s="26">
+        <v>42160</v>
+      </c>
+      <c r="AJ31" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2406,9 +2752,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
-      <c r="W32" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="W32" s="3"/>
       <c r="X32" s="5"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
@@ -2420,15 +2764,23 @@
       <c r="AF32" s="5"/>
       <c r="AG32" s="3"/>
       <c r="AH32" s="3"/>
-    </row>
-    <row r="33" spans="1:34" ht="16" thickBot="1">
-      <c r="A33" s="20" t="s">
+      <c r="AI32" s="24">
+        <v>42160</v>
+      </c>
+      <c r="AJ32" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="8"/>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="4" t="s">
         <v>1</v>
@@ -2437,18 +2789,12 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M33" s="3"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="O33" s="3"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
@@ -2456,31 +2802,35 @@
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
+      <c r="W33" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="X33" s="5"/>
       <c r="Y33" s="3"/>
-      <c r="Z33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
-      <c r="AD33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
       <c r="AF33" s="5"/>
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
-    </row>
-    <row r="34" spans="1:34" ht="16" thickBot="1">
-      <c r="A34" s="17" t="s">
+      <c r="AI33" s="25">
+        <v>42163</v>
+      </c>
+      <c r="AJ33" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="3"/>
+      <c r="B34" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="8"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
         <v>1</v>
@@ -2489,12 +2839,18 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="J34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
+      <c r="M34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
+      <c r="O34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="P34" s="5"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
@@ -2505,31 +2861,41 @@
       <c r="W34" s="3"/>
       <c r="X34" s="5"/>
       <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
+      <c r="Z34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA34" s="3"/>
       <c r="AB34" s="3"/>
       <c r="AC34" s="3"/>
-      <c r="AD34" s="3"/>
+      <c r="AD34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AE34" s="3"/>
       <c r="AF34" s="5"/>
       <c r="AG34" s="3"/>
       <c r="AH34" s="3"/>
-    </row>
-    <row r="35" spans="1:34" ht="16" thickBot="1">
-      <c r="A35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
+      <c r="AI34" s="26">
+        <v>42163</v>
+      </c>
+      <c r="AJ34" s="30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>2</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2541,9 +2907,7 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
-      <c r="T35" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="T35" s="3"/>
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
@@ -2558,70 +2922,74 @@
       <c r="AF35" s="5"/>
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
-    </row>
-    <row r="36" spans="1:34" ht="16" thickBot="1">
-      <c r="A36" s="20" t="s">
+      <c r="AI35" s="24">
+        <v>42163</v>
+      </c>
+      <c r="AJ35" s="31">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="21" t="s">
-        <v>21</v>
+      <c r="B36" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="H36" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
-      <c r="M36" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
+      <c r="T36" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="5"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
-      <c r="AA36" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AA36" s="3"/>
       <c r="AB36" s="3"/>
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
-      <c r="AE36" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE36" s="3"/>
       <c r="AF36" s="5"/>
       <c r="AG36" s="3"/>
-      <c r="AH36" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" ht="16" thickBot="1">
-      <c r="A37" s="17" t="s">
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="25">
+        <v>42167</v>
+      </c>
+      <c r="AJ36" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>2</v>
+      <c r="B37" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -2630,7 +2998,9 @@
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
+      <c r="M37" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="5"/>
@@ -2638,44 +3008,52 @@
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
-      <c r="U37" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U37" s="3"/>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="5"/>
-      <c r="Y37" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
-      <c r="AA37" s="3"/>
+      <c r="AA37" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
-      <c r="AE37" s="3"/>
+      <c r="AE37" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF37" s="5"/>
-      <c r="AG37" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH37" s="3"/>
-    </row>
-    <row r="38" spans="1:34" ht="16" thickBot="1">
-      <c r="A38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AG37" s="3"/>
+      <c r="AH37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI37" s="26">
+        <v>42167</v>
+      </c>
+      <c r="AJ37" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="F38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -2685,14 +3063,16 @@
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
-      <c r="T38" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="5"/>
-      <c r="Y38" s="3"/>
+      <c r="Y38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
@@ -2700,83 +3080,93 @@
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
       <c r="AF38" s="5"/>
-      <c r="AG38" s="3"/>
+      <c r="AG38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AH38" s="3"/>
-    </row>
-    <row r="39" spans="1:34" ht="16" thickBot="1">
-      <c r="A39" s="20" t="s">
+      <c r="AI38" s="24">
+        <v>42167</v>
+      </c>
+      <c r="AJ38" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
+      <c r="T39" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
       <c r="X39" s="5"/>
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
-      <c r="AA39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AA39" s="3"/>
       <c r="AB39" s="3"/>
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
-      <c r="AE39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE39" s="3"/>
       <c r="AF39" s="5"/>
       <c r="AG39" s="3"/>
-      <c r="AH39" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:34" ht="16" thickBot="1">
-      <c r="A40" s="17" t="s">
+      <c r="AH39" s="3"/>
+      <c r="AI39" s="25">
+        <v>42174</v>
+      </c>
+      <c r="AJ39" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>2</v>
+      <c r="B40" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="D40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E40" s="3"/>
-      <c r="F40" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="H40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="J40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
+      <c r="M40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="5"/>
@@ -2788,20 +3178,80 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
       <c r="X40" s="5"/>
-      <c r="Y40" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
+      <c r="AA40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
-      <c r="AE40" s="3"/>
+      <c r="AE40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF40" s="5"/>
-      <c r="AG40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH40" s="3"/>
+      <c r="AG40" s="3"/>
+      <c r="AH40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI40" s="26">
+        <v>42174</v>
+      </c>
+      <c r="AJ40" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="3"/>
+      <c r="AE41" s="3"/>
+      <c r="AF41" s="5"/>
+      <c r="AG41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH41" s="3"/>
+      <c r="AI41" s="24">
+        <v>42174</v>
+      </c>
+      <c r="AJ41" s="27">
+        <v>0.625</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -2821,7 +3271,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2838,7 +3288,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2850,6 +3300,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010071DB453A8FC86F4EA25EF108CEDD345F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b73adcd54c7fec9c0f197b738fe333e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4d196f5c675f743c82a55ad494504ec">
     <xsd:element name="properties">
@@ -2898,32 +3363,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48F37C0D-3141-4023-830F-4305F45374D8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5221153F-04CC-4B0F-8C35-8B7027785BDC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2937,9 +3380,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5221153F-04CC-4B0F-8C35-8B7027785BDC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48F37C0D-3141-4023-830F-4305F45374D8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Planning NLUs term 4
</commit_message>
<xml_diff>
--- a/Planning NLUs term 4.xlsx
+++ b/Planning NLUs term 4.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectDatabase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -204,6 +212,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -286,7 +297,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,8 +328,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5D9F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCC0DA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -432,6 +455,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -439,7 +484,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -507,6 +552,43 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="77"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="77"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,8 +596,36 @@
     <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFFFCCCC"/>
@@ -524,6 +634,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -816,37 +929,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AI40"/>
+  <dimension ref="A1:AK41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI40" activeCellId="3" sqref="AI25:AJ25 AI31:AJ31 AI37:AJ37 AI40:AJ40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.83203125" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="13" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="34" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="34" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="254.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:37" ht="254.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>25</v>
       </c>
@@ -951,156 +1065,228 @@
       </c>
       <c r="AI1" s="13"/>
     </row>
-    <row r="2" spans="1:35" ht="16" thickBot="1">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:37" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34">
+        <v>1</v>
+      </c>
+      <c r="D2" s="35">
+        <v>2</v>
+      </c>
+      <c r="E2" s="34">
+        <v>3</v>
+      </c>
+      <c r="F2" s="35">
+        <v>4</v>
+      </c>
+      <c r="G2" s="34">
+        <v>5</v>
+      </c>
+      <c r="H2" s="35">
+        <v>6</v>
+      </c>
+      <c r="I2" s="34">
+        <v>7</v>
+      </c>
+      <c r="J2" s="35">
+        <v>8</v>
+      </c>
+      <c r="K2" s="34">
+        <v>9</v>
+      </c>
+      <c r="L2" s="35">
+        <v>10</v>
+      </c>
+      <c r="M2" s="34">
+        <v>11</v>
+      </c>
+      <c r="N2" s="35">
+        <v>12</v>
+      </c>
+      <c r="O2" s="34">
+        <v>13</v>
+      </c>
+      <c r="P2" s="35">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="34">
+        <v>15</v>
+      </c>
+      <c r="R2" s="35">
+        <v>16</v>
+      </c>
+      <c r="S2" s="34">
+        <v>17</v>
+      </c>
+      <c r="T2" s="35">
+        <v>18</v>
+      </c>
+      <c r="U2" s="34">
+        <v>19</v>
+      </c>
+      <c r="V2" s="35">
+        <v>20</v>
+      </c>
+      <c r="W2" s="34">
+        <v>21</v>
+      </c>
+      <c r="X2" s="35">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="34">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="35">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="34">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="35">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="34">
+        <v>27</v>
+      </c>
+      <c r="AD2" s="35">
+        <v>28</v>
+      </c>
+      <c r="AE2" s="34">
+        <v>29</v>
+      </c>
+      <c r="AF2" s="35">
+        <v>30</v>
+      </c>
+      <c r="AG2" s="34">
+        <v>31</v>
+      </c>
+      <c r="AH2" s="35">
+        <v>32</v>
+      </c>
+      <c r="AI2" s="13"/>
+    </row>
+    <row r="3" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V2" s="8"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-    </row>
-    <row r="3" spans="1:35" ht="16" thickBot="1">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="M3" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="O3" s="8"/>
+      <c r="P3" s="5"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="U3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="8"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="5"/>
       <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
+      <c r="Z3" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
+      <c r="AB3" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
-      <c r="AE3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="5"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
-    </row>
-    <row r="4" spans="1:35" ht="16" thickBot="1">
-      <c r="A4" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>2</v>
+      <c r="AI3" s="24">
+        <v>42122</v>
+      </c>
+      <c r="AJ3" s="27">
+        <v>0.625</v>
+      </c>
+      <c r="AK3" s="23"/>
+    </row>
+    <row r="4" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="5"/>
+      <c r="P4" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="5"/>
+      <c r="W4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
+      <c r="AE4" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF4" s="5"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
-    </row>
-    <row r="5" spans="1:35" ht="16" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
+      <c r="AI4" s="25">
+        <v>42123</v>
+      </c>
+      <c r="AJ4" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1108,12 +1294,12 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -1130,43 +1316,43 @@
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
-      <c r="AC5" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
       <c r="AF5" s="5"/>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
-    </row>
-    <row r="6" spans="1:35" ht="16" thickBot="1">
-      <c r="A6" s="20" t="s">
+      <c r="AI5" s="24">
+        <v>42124</v>
+      </c>
+      <c r="AJ5" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>21</v>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -1178,43 +1364,53 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
+      <c r="AC6" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
       <c r="AF6" s="5"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
-    </row>
-    <row r="7" spans="1:35" ht="16" thickBot="1">
-      <c r="A7" s="17" t="s">
+      <c r="AI6" s="25">
+        <v>42125</v>
+      </c>
+      <c r="AJ6" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>2</v>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="3"/>
+      <c r="Q7" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="5"/>
@@ -1228,17 +1424,21 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
-    </row>
-    <row r="8" spans="1:35" ht="16" thickBot="1">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="AI7" s="26">
+        <v>42125</v>
+      </c>
+      <c r="AJ7" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1246,57 +1446,57 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="K8" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="R8" s="3"/>
       <c r="S8" s="3"/>
-      <c r="T8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="X8" s="5"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-      <c r="AE8" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE8" s="3"/>
       <c r="AF8" s="5"/>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
-    </row>
-    <row r="9" spans="1:35" ht="16" thickBot="1">
-      <c r="A9" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3"/>
+      <c r="AI8" s="24">
+        <v>42125</v>
+      </c>
+      <c r="AJ8" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1305,49 +1505,61 @@
       <c r="O9" s="3"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="R9" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
+      <c r="T9" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
-      <c r="X9" s="5"/>
+      <c r="X9" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Y9" s="3"/>
-      <c r="Z9" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="5"/>
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
-    </row>
-    <row r="10" spans="1:35" ht="16" thickBot="1">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
+      <c r="AI9" s="25">
+        <v>42128</v>
+      </c>
+      <c r="AJ9" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="3"/>
@@ -1359,22 +1571,32 @@
       <c r="W10" s="3"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
+      <c r="Z10" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
-      <c r="AF10" s="5"/>
+      <c r="AF10" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
-    </row>
-    <row r="11" spans="1:35" ht="16" thickBot="1">
-      <c r="A11" s="20" t="s">
+      <c r="AI10" s="24">
+        <v>42131</v>
+      </c>
+      <c r="AJ10" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>21</v>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1387,12 +1609,12 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="N11" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="O11" s="3"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -1404,19 +1626,25 @@
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
-      <c r="AC11" s="8"/>
+      <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
       <c r="AF11" s="5"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
-    </row>
-    <row r="12" spans="1:35" ht="16" thickBot="1">
-      <c r="A12" s="17" t="s">
+      <c r="AI11" s="25">
+        <v>42132</v>
+      </c>
+      <c r="AJ11" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>2</v>
+      <c r="B12" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1431,16 +1659,14 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="3"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="5"/>
@@ -1448,19 +1674,25 @@
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
+      <c r="AC12" s="8"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="5"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
-    </row>
-    <row r="13" spans="1:35" ht="16" thickBot="1">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
+      <c r="AI12" s="26">
+        <v>42132</v>
+      </c>
+      <c r="AJ12" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1470,25 +1702,21 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P13" s="5"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
+      <c r="U13" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="5"/>
@@ -1498,21 +1726,23 @@
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
-      <c r="AE13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF13" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="5"/>
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
-    </row>
-    <row r="14" spans="1:35" ht="16" thickBot="1">
-      <c r="A14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>2</v>
+      <c r="AI13" s="24">
+        <v>42132</v>
+      </c>
+      <c r="AJ13" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1522,55 +1752,61 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="K14" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="M14" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="O14" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="P14" s="5"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
+      <c r="S14" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
-      <c r="X14" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="X14" s="5"/>
       <c r="Y14" s="3"/>
-      <c r="Z14" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
-      <c r="AB14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="5"/>
+      <c r="AE14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF14" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
-    </row>
-    <row r="15" spans="1:35" ht="16" thickBot="1">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
+      <c r="AI14" s="25">
+        <v>42135</v>
+      </c>
+      <c r="AJ14" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1583,58 +1819,72 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
-      <c r="W15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="X15" s="5"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
+      <c r="Z15" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
+      <c r="AB15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
       <c r="AF15" s="5"/>
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
-    </row>
-    <row r="16" spans="1:35" ht="16" thickBot="1">
+      <c r="AI15" s="24">
+        <v>42136</v>
+      </c>
+      <c r="AJ15" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="T16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
+      <c r="W16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="X16" s="5"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
@@ -1646,45 +1896,41 @@
       <c r="AF16" s="5"/>
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
-    </row>
-    <row r="17" spans="1:34" ht="16" thickBot="1">
-      <c r="A17" s="20" t="s">
+      <c r="AI16" s="25">
+        <v>42137</v>
+      </c>
+      <c r="AJ16" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="N17" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="O17" s="3"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -1693,65 +1939,85 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
       <c r="AF17" s="5"/>
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
-    </row>
-    <row r="18" spans="1:34" ht="16" thickBot="1">
-      <c r="A18" s="17" t="s">
+      <c r="AI17" s="25">
+        <v>42146</v>
+      </c>
+      <c r="AJ17" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
+      <c r="AB18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="5"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
-    </row>
-    <row r="19" spans="1:34" ht="16" thickBot="1">
+      <c r="AI18" s="26">
+        <v>42146</v>
+      </c>
+      <c r="AJ18" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>2</v>
@@ -1762,132 +2028,138 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="K19" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L19" s="3"/>
-      <c r="M19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="5"/>
+      <c r="P19" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
-      <c r="AF19" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="AF19" s="5"/>
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
-    </row>
-    <row r="20" spans="1:34" ht="16" thickBot="1">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
+      <c r="AI19" s="24">
+        <v>42146</v>
+      </c>
+      <c r="AJ19" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" s="3"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
+      <c r="V20" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="W20" s="3"/>
-      <c r="X20" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="X20" s="5"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
+      <c r="Z20" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
       <c r="AE20" s="3"/>
-      <c r="AF20" s="5"/>
+      <c r="AF20" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
-    </row>
-    <row r="21" spans="1:34" ht="16" thickBot="1">
-      <c r="A21" s="20" t="s">
+      <c r="AI20" s="24">
+        <v>42152</v>
+      </c>
+      <c r="AJ20" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
+      <c r="O21" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="P21" s="5"/>
-      <c r="Q21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
-      <c r="X21" s="5"/>
+      <c r="X21" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
@@ -1898,39 +2170,51 @@
       <c r="AF21" s="5"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
-    </row>
-    <row r="22" spans="1:34" ht="16" thickBot="1">
-      <c r="A22" s="17" t="s">
+      <c r="AI21" s="25">
+        <v>42153</v>
+      </c>
+      <c r="AJ21" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="B22" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="F22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
-      <c r="U22" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="5"/>
@@ -1944,62 +2228,76 @@
       <c r="AF22" s="5"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
-    </row>
-    <row r="23" spans="1:34" ht="16" thickBot="1">
-      <c r="A23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
+      <c r="AI22" s="26">
+        <v>42153</v>
+      </c>
+      <c r="AJ22" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="5"/>
+      <c r="P23" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
+      <c r="U23" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="5"/>
       <c r="Y23" s="3"/>
-      <c r="Z23" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
-      <c r="AD23" s="8"/>
-      <c r="AE23" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
       <c r="AF23" s="5"/>
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
-    </row>
-    <row r="24" spans="1:34" ht="16" thickBot="1">
-      <c r="A24" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>2</v>
+      <c r="AI23" s="24">
+        <v>42153</v>
+      </c>
+      <c r="AJ23" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -2016,35 +2314,37 @@
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
-      <c r="U24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V24" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
-      <c r="AD24" s="3"/>
-      <c r="AE24" s="3"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF24" s="5"/>
       <c r="AG24" s="3"/>
-      <c r="AH24" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" ht="16" thickBot="1">
-      <c r="A25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>4</v>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="25">
+        <v>42156</v>
+      </c>
+      <c r="AJ24" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2064,41 +2364,45 @@
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W25" s="3"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="3"/>
-      <c r="Z25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
-      <c r="AD25" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
       <c r="AF25" s="5"/>
       <c r="AG25" s="3"/>
-      <c r="AH25" s="3"/>
-    </row>
-    <row r="26" spans="1:34" ht="16" thickBot="1">
+      <c r="AH25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="24">
+        <v>42157</v>
+      </c>
+      <c r="AJ25" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -2116,32 +2420,42 @@
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
+      <c r="W26" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="X26" s="5"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
+      <c r="Z26" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
+      <c r="AD26" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AE26" s="3"/>
       <c r="AF26" s="5"/>
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
-    </row>
-    <row r="27" spans="1:34" ht="16" thickBot="1">
-      <c r="A27" s="20" t="s">
+      <c r="AI26" s="25">
+        <v>42158</v>
+      </c>
+      <c r="AJ26" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>21</v>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="4" t="s">
         <v>1</v>
       </c>
@@ -2152,13 +2466,9 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="O27" s="3"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
@@ -2174,24 +2484,30 @@
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
-      <c r="AE27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE27" s="3"/>
       <c r="AF27" s="5"/>
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
-    </row>
-    <row r="28" spans="1:34" ht="16" thickBot="1">
-      <c r="A28" s="17" t="s">
+      <c r="AI27" s="25">
+        <v>42159</v>
+      </c>
+      <c r="AJ27" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>2</v>
+      <c r="B28" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E28" s="4" t="s">
         <v>1</v>
       </c>
@@ -2202,43 +2518,47 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O28" s="3"/>
+      <c r="M28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="P28" s="5"/>
       <c r="Q28" s="3"/>
-      <c r="R28" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
-      <c r="V28" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="5"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
-      <c r="AB28" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
-      <c r="AE28" s="3"/>
+      <c r="AE28" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF28" s="5"/>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
-    </row>
-    <row r="29" spans="1:34" ht="16" thickBot="1">
-      <c r="A29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
+      <c r="AI28" s="26">
+        <v>42159</v>
+      </c>
+      <c r="AJ28" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>1</v>
@@ -2255,40 +2575,48 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="8"/>
+      <c r="N29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O29" s="3"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="R29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
       <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
+      <c r="V29" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="W29" s="3"/>
       <c r="X29" s="5"/>
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
+      <c r="AB29" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AC29" s="3"/>
-      <c r="AD29" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
       <c r="AF29" s="5"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
-    </row>
-    <row r="30" spans="1:34" ht="16" thickBot="1">
-      <c r="A30" s="20" t="s">
+      <c r="AI29" s="24">
+        <v>42159</v>
+      </c>
+      <c r="AJ29" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>21</v>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>1</v>
@@ -2301,55 +2629,65 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
+      <c r="O30" s="8"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
+      <c r="S30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="5"/>
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
-      <c r="AA30" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
-      <c r="AD30" s="3"/>
+      <c r="AD30" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AE30" s="3"/>
       <c r="AF30" s="5"/>
       <c r="AG30" s="3"/>
-      <c r="AH30" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:34" ht="16" thickBot="1">
-      <c r="A31" s="17" t="s">
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="25">
+        <v>42160</v>
+      </c>
+      <c r="AJ30" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>2</v>
+      <c r="B31" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="E31" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="J31" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -2366,29 +2704,37 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
+      <c r="AA31" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
       <c r="AE31" s="3"/>
       <c r="AF31" s="5"/>
       <c r="AG31" s="3"/>
-      <c r="AH31" s="3"/>
-    </row>
-    <row r="32" spans="1:34" ht="16" thickBot="1">
-      <c r="A32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
+      <c r="AH31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI31" s="26">
+        <v>42160</v>
+      </c>
+      <c r="AJ31" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2406,9 +2752,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
-      <c r="W32" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="W32" s="3"/>
       <c r="X32" s="5"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
@@ -2420,15 +2764,23 @@
       <c r="AF32" s="5"/>
       <c r="AG32" s="3"/>
       <c r="AH32" s="3"/>
-    </row>
-    <row r="33" spans="1:34" ht="16" thickBot="1">
-      <c r="A33" s="20" t="s">
+      <c r="AI32" s="24">
+        <v>42160</v>
+      </c>
+      <c r="AJ32" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="8"/>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="4" t="s">
         <v>1</v>
@@ -2437,18 +2789,12 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M33" s="3"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="O33" s="3"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
@@ -2456,31 +2802,35 @@
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
+      <c r="W33" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="X33" s="5"/>
       <c r="Y33" s="3"/>
-      <c r="Z33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
-      <c r="AD33" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
       <c r="AF33" s="5"/>
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
-    </row>
-    <row r="34" spans="1:34" ht="16" thickBot="1">
-      <c r="A34" s="17" t="s">
+      <c r="AI33" s="25">
+        <v>42163</v>
+      </c>
+      <c r="AJ33" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="3"/>
+      <c r="B34" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="8"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4" t="s">
         <v>1</v>
@@ -2489,12 +2839,18 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="J34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
+      <c r="M34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
+      <c r="O34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="P34" s="5"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
@@ -2505,31 +2861,41 @@
       <c r="W34" s="3"/>
       <c r="X34" s="5"/>
       <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
+      <c r="Z34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AA34" s="3"/>
       <c r="AB34" s="3"/>
       <c r="AC34" s="3"/>
-      <c r="AD34" s="3"/>
+      <c r="AD34" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AE34" s="3"/>
       <c r="AF34" s="5"/>
       <c r="AG34" s="3"/>
       <c r="AH34" s="3"/>
-    </row>
-    <row r="35" spans="1:34" ht="16" thickBot="1">
-      <c r="A35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
+      <c r="AI34" s="26">
+        <v>42163</v>
+      </c>
+      <c r="AJ34" s="30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>2</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2541,9 +2907,7 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
-      <c r="T35" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="T35" s="3"/>
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
@@ -2558,70 +2922,74 @@
       <c r="AF35" s="5"/>
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
-    </row>
-    <row r="36" spans="1:34" ht="16" thickBot="1">
-      <c r="A36" s="20" t="s">
+      <c r="AI35" s="24">
+        <v>42163</v>
+      </c>
+      <c r="AJ35" s="31">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="21" t="s">
-        <v>21</v>
+      <c r="B36" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="H36" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
-      <c r="M36" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
+      <c r="T36" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="5"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
-      <c r="AA36" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AA36" s="3"/>
       <c r="AB36" s="3"/>
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
-      <c r="AE36" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE36" s="3"/>
       <c r="AF36" s="5"/>
       <c r="AG36" s="3"/>
-      <c r="AH36" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" ht="16" thickBot="1">
-      <c r="A37" s="17" t="s">
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="25">
+        <v>42167</v>
+      </c>
+      <c r="AJ36" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>2</v>
+      <c r="B37" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -2630,7 +2998,9 @@
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
+      <c r="M37" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="5"/>
@@ -2638,44 +3008,52 @@
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
-      <c r="U37" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="U37" s="3"/>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="5"/>
-      <c r="Y37" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
-      <c r="AA37" s="3"/>
+      <c r="AA37" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
-      <c r="AE37" s="3"/>
+      <c r="AE37" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF37" s="5"/>
-      <c r="AG37" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH37" s="3"/>
-    </row>
-    <row r="38" spans="1:34" ht="16" thickBot="1">
-      <c r="A38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AG37" s="3"/>
+      <c r="AH37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI37" s="26">
+        <v>42167</v>
+      </c>
+      <c r="AJ37" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="F38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -2685,14 +3063,16 @@
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
-      <c r="T38" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="5"/>
-      <c r="Y38" s="3"/>
+      <c r="Y38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
@@ -2700,83 +3080,93 @@
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
       <c r="AF38" s="5"/>
-      <c r="AG38" s="3"/>
+      <c r="AG38" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AH38" s="3"/>
-    </row>
-    <row r="39" spans="1:34" ht="16" thickBot="1">
-      <c r="A39" s="20" t="s">
+      <c r="AI38" s="24">
+        <v>42167</v>
+      </c>
+      <c r="AJ38" s="27">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
+      <c r="T39" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
       <c r="X39" s="5"/>
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
-      <c r="AA39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AA39" s="3"/>
       <c r="AB39" s="3"/>
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
-      <c r="AE39" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="AE39" s="3"/>
       <c r="AF39" s="5"/>
       <c r="AG39" s="3"/>
-      <c r="AH39" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:34" ht="16" thickBot="1">
-      <c r="A40" s="17" t="s">
+      <c r="AH39" s="3"/>
+      <c r="AI39" s="25">
+        <v>42174</v>
+      </c>
+      <c r="AJ39" s="28">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>2</v>
+      <c r="B40" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="D40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E40" s="3"/>
-      <c r="F40" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="H40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="J40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
+      <c r="M40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="5"/>
@@ -2788,20 +3178,80 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
       <c r="X40" s="5"/>
-      <c r="Y40" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
+      <c r="AA40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
-      <c r="AE40" s="3"/>
+      <c r="AE40" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="AF40" s="5"/>
-      <c r="AG40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH40" s="3"/>
+      <c r="AG40" s="3"/>
+      <c r="AH40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI40" s="26">
+        <v>42174</v>
+      </c>
+      <c r="AJ40" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="3"/>
+      <c r="AE41" s="3"/>
+      <c r="AF41" s="5"/>
+      <c r="AG41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH41" s="3"/>
+      <c r="AI41" s="24">
+        <v>42174</v>
+      </c>
+      <c r="AJ41" s="27">
+        <v>0.625</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -2821,7 +3271,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2838,7 +3288,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2850,6 +3300,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010071DB453A8FC86F4EA25EF108CEDD345F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b73adcd54c7fec9c0f197b738fe333e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4d196f5c675f743c82a55ad494504ec">
     <xsd:element name="properties">
@@ -2898,32 +3363,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48F37C0D-3141-4023-830F-4305F45374D8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5221153F-04CC-4B0F-8C35-8B7027785BDC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2937,9 +3380,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5221153F-04CC-4B0F-8C35-8B7027785BDC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48F37C0D-3141-4023-830F-4305F45374D8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>